<commit_message>
Update Abbot & von Doenhoff comparison.xlsx
</commit_message>
<xml_diff>
--- a/Abbot & von Doenhoff comparison.xlsx
+++ b/Abbot & von Doenhoff comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eden\Documents\GitHub\AerodynamicsOfWingsAndBodies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lior\Documents\GitHub\AerodynamicsOfWingsAndBodies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19267803-369B-44C9-B92D-BDC28A8375B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B151CB65-B7EA-442C-AF48-8574D42C1AEC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="11244" xr2:uid="{62AF0D42-47B3-4C56-9EF3-63E5043B7993}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="11250" xr2:uid="{62AF0D42-47B3-4C56-9EF3-63E5043B7993}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -415,21 +415,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,27 +465,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-54.65281185149378</v>
+        <v>581.81184391588317</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>54.65281185149378</v>
+        <v>581.81184391588317</v>
       </c>
       <c r="E2">
-        <v>0.70130701567252207</v>
+        <v>-32.850502172080006</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.29869298432747793</v>
+        <v>33.850502172080006</v>
       </c>
       <c r="H2">
         <v>65535</v>
@@ -493,628 +494,628 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.54652811851493777</v>
+        <v>5.8181184391588321</v>
       </c>
       <c r="K2">
         <v>65535</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B3">
-        <v>52.324526449191012</v>
+        <v>52.468904602940491</v>
       </c>
       <c r="C3">
-        <v>61.841621472089528</v>
+        <v>62.015268114861158</v>
       </c>
       <c r="D3">
-        <v>81.007667627387562</v>
+        <v>81.23348711947915</v>
       </c>
       <c r="E3">
-        <v>0.34377577855707064</v>
+        <v>0.3401120570409415</v>
       </c>
       <c r="F3">
         <v>0.64</v>
       </c>
       <c r="G3">
-        <v>0.65622422144292936</v>
+        <v>0.6598879429590585</v>
       </c>
       <c r="H3">
-        <v>2.5350346004577098E-2</v>
+        <v>3.1074910873528892E-2</v>
       </c>
       <c r="I3">
         <v>0.8</v>
       </c>
       <c r="J3">
-        <v>0.81007667627387558</v>
+        <v>0.81233487119479153</v>
       </c>
       <c r="K3">
-        <v>1.2595845342344425E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.5418588993489357E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="B4">
-        <v>82.066434143825234</v>
+        <v>82.103732443261279</v>
       </c>
       <c r="C4">
-        <v>58.749736581416713</v>
+        <v>58.775745317600325</v>
       </c>
       <c r="D4">
-        <v>100.92785126747056</v>
+        <v>100.97331884589143</v>
       </c>
       <c r="E4">
-        <v>-1.8643116146865868E-2</v>
+        <v>-1.9561111875405102E-2</v>
       </c>
       <c r="F4">
         <v>1.01</v>
       </c>
       <c r="G4">
-        <v>1.0186431161468659</v>
+        <v>1.0195611118754051</v>
       </c>
       <c r="H4">
-        <v>8.5575407394711481E-3</v>
+        <v>9.4664474013911801E-3</v>
       </c>
       <c r="I4">
         <v>1.0049999999999999</v>
       </c>
       <c r="J4">
-        <v>1.0092785126747055</v>
+        <v>1.0097331884589142</v>
       </c>
       <c r="K4">
-        <v>4.257226541995604E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4.70964025762622E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="B5">
-        <v>100.20558274210197</v>
+        <v>100.21699723365364</v>
       </c>
       <c r="C5">
-        <v>47.847768816351497</v>
+        <v>47.853232711935554</v>
       </c>
       <c r="D5">
-        <v>111.0430898047567</v>
+        <v>111.05574463085105</v>
       </c>
       <c r="E5">
-        <v>-0.23305677933872615</v>
+        <v>-0.23333784155128012</v>
       </c>
       <c r="F5">
         <v>1.2410000000000001</v>
       </c>
       <c r="G5">
-        <v>1.2330567793387261</v>
+        <v>1.2333378415512801</v>
       </c>
       <c r="H5">
-        <v>6.4006612903093896E-3</v>
+        <v>6.1741808611764544E-3</v>
       </c>
       <c r="I5">
         <v>1.1140000000000001</v>
       </c>
       <c r="J5">
-        <v>1.110430898047567</v>
+        <v>1.1105574463085106</v>
       </c>
       <c r="K5">
-        <v>3.2038617167262974E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3.090263636884642E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.05</v>
       </c>
       <c r="B6">
-        <v>111.67031653327584</v>
+        <v>111.67353020854374</v>
       </c>
       <c r="C6">
-        <v>33.823372169484564</v>
+        <v>33.824354399947424</v>
       </c>
       <c r="D6">
-        <v>116.68024725529803</v>
+        <v>116.68360767396496</v>
       </c>
       <c r="E6">
-        <v>-0.36142800995574809</v>
+        <v>-0.36150642998117721</v>
       </c>
       <c r="F6">
         <v>1.3779999999999999</v>
       </c>
       <c r="G6">
-        <v>1.3614280099557481</v>
+        <v>1.3615064299811772</v>
       </c>
       <c r="H6">
-        <v>1.2026117593796667E-2</v>
+        <v>1.196920901220804E-2</v>
       </c>
       <c r="I6">
         <v>1.1739999999999999</v>
       </c>
       <c r="J6">
-        <v>1.1668024725529802</v>
+        <v>1.1668360767396495</v>
       </c>
       <c r="K6">
-        <v>6.1307729531684292E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>6.1021492847959328E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="B7">
-        <v>115.51962713971938</v>
+        <v>115.52112660204648</v>
       </c>
       <c r="C7">
-        <v>25.503210820357303</v>
+        <v>25.503532510051429</v>
       </c>
       <c r="D7">
-        <v>118.30130183834571</v>
+        <v>118.30283539246767</v>
       </c>
       <c r="E7">
-        <v>-0.39951980166473788</v>
+        <v>-0.39955608618973026</v>
       </c>
       <c r="F7">
         <v>1.4019999999999999</v>
       </c>
       <c r="G7">
-        <v>1.3995198016647379</v>
+        <v>1.3995560861897303</v>
       </c>
       <c r="H7">
-        <v>1.7690430351369683E-3</v>
+        <v>1.7431624894933303E-3</v>
       </c>
       <c r="I7">
         <v>1.1839999999999999</v>
       </c>
       <c r="J7">
-        <v>1.1830130183834571</v>
+        <v>1.1830283539246766</v>
       </c>
       <c r="K7">
-        <v>8.3359933829634317E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>8.2064702307710802E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.1</v>
       </c>
       <c r="B8">
-        <v>117.16336636985736</v>
+        <v>117.16422706548609</v>
       </c>
       <c r="C8">
-        <v>19.770827087331895</v>
+        <v>19.770979568610642</v>
       </c>
       <c r="D8">
-        <v>118.81977959428556</v>
+        <v>118.82065366322136</v>
       </c>
       <c r="E8">
-        <v>-0.41181400228345999</v>
+        <v>-0.41183477369552013</v>
       </c>
       <c r="F8">
         <v>1.411</v>
       </c>
       <c r="G8">
-        <v>1.41181400228346</v>
+        <v>1.4118347736955201</v>
       </c>
       <c r="H8">
-        <v>5.768974368957888E-4</v>
+        <v>5.9161849434450514E-4</v>
       </c>
       <c r="I8">
         <v>1.1879999999999999</v>
       </c>
       <c r="J8">
-        <v>1.1881977959428556</v>
+        <v>1.1882065366322137</v>
       </c>
       <c r="K8">
-        <v>1.6649490139362586E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.7385238401827039E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.15</v>
       </c>
       <c r="B9">
-        <v>118.07189934393962</v>
+        <v>118.07231132749567</v>
       </c>
       <c r="C9">
-        <v>12.017562125060437</v>
+        <v>12.017606603073391</v>
       </c>
       <c r="D9">
-        <v>118.68190769496039</v>
+        <v>118.68232206475949</v>
       </c>
       <c r="E9">
-        <v>-0.40853952141150973</v>
+        <v>-0.40854935706832962</v>
       </c>
       <c r="F9">
         <v>1.411</v>
       </c>
       <c r="G9">
-        <v>1.4085395214115097</v>
+        <v>1.4085493570683296</v>
       </c>
       <c r="H9">
-        <v>1.743783549603331E-3</v>
+        <v>1.7368128502270803E-3</v>
       </c>
       <c r="I9">
         <v>1.1879999999999999</v>
       </c>
       <c r="J9">
-        <v>1.1868190769496039</v>
+        <v>1.1868232206475948</v>
       </c>
       <c r="K9">
-        <v>9.9404297171386919E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9.9055501044202176E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.2</v>
       </c>
       <c r="B10">
-        <v>117.71315442358727</v>
+        <v>117.71340178360596</v>
       </c>
       <c r="C10">
-        <v>6.7924440362983489</v>
+        <v>6.7924605369065594</v>
       </c>
       <c r="D10">
-        <v>117.90896497017327</v>
+        <v>117.90921286996227</v>
       </c>
       <c r="E10">
-        <v>-0.39025240203375477</v>
+        <v>-0.39025824796140784</v>
       </c>
       <c r="F10">
         <v>1.399</v>
       </c>
       <c r="G10">
-        <v>1.3902524020337548</v>
+        <v>1.3902582479614078</v>
       </c>
       <c r="H10">
-        <v>6.2527505119694396E-3</v>
+        <v>6.2485718646119919E-3</v>
       </c>
       <c r="I10">
         <v>1.1830000000000001</v>
       </c>
       <c r="J10">
-        <v>1.1790896497017327</v>
+        <v>1.1790921286996228</v>
       </c>
       <c r="K10">
-        <v>3.3054524921955724E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3.3033569741143581E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.25</v>
       </c>
       <c r="B11">
-        <v>116.8239142644542</v>
+        <v>116.82407772165713</v>
       </c>
       <c r="C11">
-        <v>2.9483331604094101</v>
+        <v>2.9483476615003887</v>
       </c>
       <c r="D11">
-        <v>116.8611124903974</v>
+        <v>116.86127626142401</v>
       </c>
       <c r="E11">
-        <v>-0.36565196124933164</v>
+        <v>-0.36565578894488637</v>
       </c>
       <c r="F11">
         <v>1.3779999999999999</v>
       </c>
       <c r="G11">
-        <v>1.3656519612493316</v>
+        <v>1.3656557889448864</v>
       </c>
       <c r="H11">
-        <v>8.9608408930829143E-3</v>
+        <v>8.9580631749735257E-3</v>
       </c>
       <c r="I11">
         <v>1.1739999999999999</v>
       </c>
       <c r="J11">
-        <v>1.1686111249039741</v>
+        <v>1.1686127626142402</v>
       </c>
       <c r="K11">
-        <v>4.5901832163763321E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4.5887882331854743E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.3</v>
       </c>
       <c r="B12">
-        <v>115.67551243642924</v>
+        <v>115.67562454978497</v>
       </c>
       <c r="C12">
-        <v>-8.9865414411383297E-3</v>
+        <v>-8.9964029785963243E-3</v>
       </c>
       <c r="D12">
-        <v>115.67551278550022</v>
+        <v>115.67562489962214</v>
       </c>
       <c r="E12">
-        <v>-0.3380824258188424</v>
+        <v>-0.33808501959180814</v>
       </c>
       <c r="F12">
         <v>1.35</v>
       </c>
       <c r="G12">
-        <v>1.3380824258188424</v>
+        <v>1.3380850195918081</v>
       </c>
       <c r="H12">
-        <v>8.8278327267834709E-3</v>
+        <v>8.825911413475513E-3</v>
       </c>
       <c r="I12">
         <v>1.1619999999999999</v>
       </c>
       <c r="J12">
-        <v>1.1567551278550021</v>
+        <v>1.1567562489962213</v>
       </c>
       <c r="K12">
-        <v>4.5136593330445812E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4.5126944955065466E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.4</v>
       </c>
       <c r="B13">
-        <v>113.05696706761981</v>
+        <v>113.05698777479228</v>
       </c>
       <c r="C13">
-        <v>-4.2111992074067155</v>
+        <v>-4.2111426559548653</v>
       </c>
       <c r="D13">
-        <v>113.13537024862443</v>
+        <v>113.13538883646589</v>
       </c>
       <c r="E13">
-        <v>-0.27996120012933323</v>
+        <v>-0.27996162071783304</v>
       </c>
       <c r="F13">
         <v>1.288</v>
       </c>
       <c r="G13">
-        <v>1.2799612001293332</v>
+        <v>1.279961620717833</v>
       </c>
       <c r="H13">
-        <v>6.241304247412113E-3</v>
+        <v>6.2409777035458041E-3</v>
       </c>
       <c r="I13">
         <v>1.135</v>
       </c>
       <c r="J13">
-        <v>1.1313537024862443</v>
+        <v>1.131353888364659</v>
       </c>
       <c r="K13">
-        <v>3.2125969284190923E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3.2124331588907571E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.5</v>
       </c>
       <c r="B14">
-        <v>110.33295749198177</v>
+        <v>110.33311265053909</v>
       </c>
       <c r="C14">
-        <v>-6.9636641962750572</v>
+        <v>-6.963232862893924</v>
       </c>
       <c r="D14">
-        <v>110.55249489706662</v>
+        <v>110.55262257883997</v>
       </c>
       <c r="E14">
-        <v>-0.2221854127965941</v>
+        <v>-0.22218823590594372</v>
       </c>
       <c r="F14">
         <v>1.228</v>
       </c>
       <c r="G14">
-        <v>1.2221854127965941</v>
+        <v>1.2221882359059437</v>
       </c>
       <c r="H14">
-        <v>4.735005865965705E-3</v>
+        <v>4.7327069169839251E-3</v>
       </c>
       <c r="I14">
         <v>1.1080000000000001</v>
       </c>
       <c r="J14">
-        <v>1.1055249489706662</v>
+        <v>1.1055262257883998</v>
       </c>
       <c r="K14">
-        <v>2.2338005679908611E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2.2326482054154623E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.6</v>
       </c>
       <c r="B15">
-        <v>107.62464618507555</v>
+        <v>107.62656484123201</v>
       </c>
       <c r="C15">
-        <v>-8.8424548223020025</v>
+        <v>-8.8419875975868418</v>
       </c>
       <c r="D15">
-        <v>107.9872838520682</v>
+        <v>107.98915780854945</v>
       </c>
       <c r="E15">
-        <v>-0.16612534737471485</v>
+        <v>-0.16616582041997963</v>
       </c>
       <c r="F15">
         <v>1.1659999999999999</v>
       </c>
       <c r="G15">
-        <v>1.1661253473747148</v>
+        <v>1.1661658204199796</v>
       </c>
       <c r="H15">
-        <v>1.0750203663372524E-4</v>
+        <v>1.4221305315583266E-4</v>
       </c>
       <c r="I15">
         <v>1.08</v>
       </c>
       <c r="J15">
-        <v>1.0798728385206819</v>
+        <v>1.0798915780854945</v>
       </c>
       <c r="K15">
-        <v>1.1774211047974766E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.0039066157921485E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.7</v>
       </c>
       <c r="B16">
-        <v>104.87682885407472</v>
+        <v>104.87491866295302</v>
       </c>
       <c r="C16">
-        <v>-10.195589178553185</v>
+        <v>-10.202988149107831</v>
       </c>
       <c r="D16">
-        <v>105.37124498260761</v>
+        <v>105.37005993987023</v>
       </c>
       <c r="E16">
-        <v>-0.11030992691847086</v>
+        <v>-0.11028495317318465</v>
       </c>
       <c r="F16">
         <v>1.109</v>
       </c>
       <c r="G16">
-        <v>1.1103099269184709</v>
+        <v>1.1102849531731847</v>
       </c>
       <c r="H16">
-        <v>1.1811784657086309E-3</v>
+        <v>1.1586593085524495E-3</v>
       </c>
       <c r="I16">
         <v>1.0529999999999999</v>
       </c>
       <c r="J16">
-        <v>1.0537124498260761</v>
+        <v>1.0537005993987023</v>
       </c>
       <c r="K16">
-        <v>6.7659052808757012E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>6.6533656097091446E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.8</v>
       </c>
       <c r="B17">
-        <v>101.77348242558035</v>
+        <v>101.80826909238152</v>
       </c>
       <c r="C17">
-        <v>-11.277467480128008</v>
+        <v>-11.276470728167068</v>
       </c>
       <c r="D17">
-        <v>102.39640129318637</v>
+        <v>102.43086667440618</v>
       </c>
       <c r="E17">
-        <v>-4.8502299779525915E-2</v>
+        <v>-4.9208244766997478E-2</v>
       </c>
       <c r="F17">
         <v>1.044</v>
       </c>
       <c r="G17">
-        <v>1.0485022997795259</v>
+        <v>1.0492082447669975</v>
       </c>
       <c r="H17">
-        <v>4.3125476815381947E-3</v>
+        <v>4.9887401982734083E-3</v>
       </c>
       <c r="I17">
         <v>1.022</v>
       </c>
       <c r="J17">
-        <v>1.0239640129318637</v>
+        <v>1.0243086667440617</v>
       </c>
       <c r="K17">
-        <v>1.9217347669898794E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2.2589694168901331E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.9</v>
       </c>
       <c r="B18">
-        <v>97.83431080020884</v>
+        <v>97.632286567408542</v>
       </c>
       <c r="C18">
-        <v>-12.186614226689658</v>
+        <v>-12.155052156447296</v>
       </c>
       <c r="D18">
-        <v>98.590394745441685</v>
+        <v>98.386018688157804</v>
       </c>
       <c r="E18">
-        <v>2.7993406393798437E-2</v>
+        <v>3.2019132669346306E-2</v>
       </c>
       <c r="F18">
         <v>0.95599999999999996</v>
       </c>
       <c r="G18">
-        <v>0.97200659360620156</v>
+        <v>0.96798086733065369</v>
       </c>
       <c r="H18">
-        <v>1.6743298751256908E-2</v>
+        <v>1.2532288002775872E-2</v>
       </c>
       <c r="I18">
         <v>0.97799999999999998</v>
       </c>
       <c r="J18">
-        <v>0.9859039474544169</v>
+        <v>0.98386018688157806</v>
       </c>
       <c r="K18">
-        <v>8.0817458634119786E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>5.992011126357953E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.95</v>
       </c>
       <c r="B19">
-        <v>94.741781171972391</v>
+        <v>94.259165602612342</v>
       </c>
       <c r="C19">
-        <v>-12.8523731673959</v>
+        <v>-12.442818184847773</v>
       </c>
       <c r="D19">
-        <v>95.609563306564169</v>
+        <v>95.076884806360141</v>
       </c>
       <c r="E19">
-        <v>8.588114043280981E-2</v>
+        <v>9.6038597551812432E-2</v>
       </c>
       <c r="F19">
         <v>0.90600000000000003</v>
       </c>
       <c r="G19">
-        <v>0.91411885956719019</v>
+        <v>0.90396140244818757</v>
       </c>
       <c r="H19">
-        <v>8.9612136503202672E-3</v>
+        <v>2.2501076730821854E-3</v>
       </c>
       <c r="I19">
         <v>0.95199999999999996</v>
       </c>
       <c r="J19">
-        <v>0.95609563306564171</v>
+        <v>0.9507688480636014</v>
       </c>
       <c r="K19">
-        <v>4.3021355731531069E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.2932268239480627E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>62.41517027226584</v>
+        <v>69.849837469570758</v>
       </c>
       <c r="C20">
-        <v>-35.481499604171432</v>
+        <v>-45.513414731382063</v>
       </c>
       <c r="D20">
-        <v>71.795475444325561</v>
+        <v>83.369483116043341</v>
       </c>
       <c r="E20">
-        <v>0.48454097057232448</v>
+        <v>0.30495292849637634</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.51545902942767552</v>
+        <v>0.69504707150362366</v>
       </c>
       <c r="H20">
         <v>65535</v>
@@ -1123,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.71795475444325563</v>
+        <v>0.83369483116043341</v>
       </c>
       <c r="K20">
         <v>65535</v>
@@ -1140,7 +1141,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1152,7 +1153,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>